<commit_message>
fix bug kdr003  #117682
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KDR003_template.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KDR003_template.xlsx
@@ -11,16 +11,15 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'振休確認表(日数管理_紐付あり_年月日)'!$A$2:$S$19</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'振休確認表(日数管理_紐付あり_年月日)'!$A$1:$S$19</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'振休確認表(日数管理_紐付あり_年月日)'!$1:$3</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -47,19 +46,6 @@
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <name val="ＭＳ ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FFFF0000"/>
-      <name val="ＭＳ ゴシック"/>
-      <family val="3"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -520,7 +506,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -644,122 +630,74 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="2" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="5" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="2" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="2" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="5" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="5" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
@@ -812,11 +750,47 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="2" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1093,15 +1067,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="145" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="9.75"/>
   <cols>
     <col min="1" max="1" width="3.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.25" style="2" customWidth="1"/>
     <col min="3" max="7" width="5.875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="2.5" style="2" customWidth="1"/>
-    <col min="9" max="9" width="5.125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="2.5" style="90" customWidth="1"/>
+    <col min="9" max="9" width="5.125" style="90" customWidth="1"/>
     <col min="10" max="19" width="7.875" style="3" customWidth="1"/>
     <col min="20" max="20" width="9" style="1"/>
     <col min="21" max="16384" width="9" style="2"/>
@@ -1115,83 +1089,83 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="81"/>
-      <c r="R1" s="81"/>
-      <c r="S1" s="81"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
     </row>
     <row r="2" spans="1:20" ht="11.25" customHeight="1">
-      <c r="A2" s="85"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="76"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="83"/>
       <c r="T2" s="30"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="86"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="79"/>
-      <c r="S3" s="77"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="82"/>
+      <c r="R3" s="82"/>
+      <c r="S3" s="84"/>
       <c r="T3" s="30"/>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="82"/>
-      <c r="B4" s="83"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="83"/>
-      <c r="P4" s="83"/>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="83"/>
-      <c r="S4" s="84"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="67"/>
+      <c r="O4" s="67"/>
+      <c r="P4" s="67"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="68"/>
       <c r="T4" s="30"/>
     </row>
     <row r="5" spans="1:20">
@@ -1459,266 +1433,278 @@
       <c r="T16" s="30"/>
     </row>
     <row r="17" spans="1:20">
-      <c r="A17" s="41"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="46"/>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="46"/>
-      <c r="R17" s="47"/>
-      <c r="S17" s="47"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="85"/>
+      <c r="I17" s="91"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="39"/>
+      <c r="S17" s="39"/>
       <c r="T17" s="30"/>
     </row>
     <row r="18" spans="1:20">
-      <c r="A18" s="48"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="53"/>
-      <c r="P18" s="53"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="54"/>
-      <c r="S18" s="54"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="86"/>
+      <c r="I18" s="92"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="44"/>
+      <c r="N18" s="44"/>
+      <c r="O18" s="44"/>
+      <c r="P18" s="44"/>
+      <c r="Q18" s="44"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="45"/>
       <c r="T18" s="30"/>
     </row>
     <row r="19" spans="1:20">
-      <c r="A19" s="55"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="61"/>
-      <c r="N19" s="61"/>
-      <c r="O19" s="61"/>
-      <c r="P19" s="61"/>
-      <c r="Q19" s="61"/>
-      <c r="R19" s="62"/>
-      <c r="S19" s="62"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="87"/>
+      <c r="I19" s="93"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="52"/>
+      <c r="Q19" s="52"/>
+      <c r="R19" s="53"/>
+      <c r="S19" s="53"/>
       <c r="T19" s="30"/>
     </row>
     <row r="20" spans="1:20">
-      <c r="A20" s="55"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="75"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="63"/>
-      <c r="K20" s="63"/>
-      <c r="L20" s="63"/>
-      <c r="M20" s="63"/>
-      <c r="N20" s="63"/>
-      <c r="O20" s="63"/>
-      <c r="P20" s="63"/>
-      <c r="Q20" s="63"/>
-      <c r="R20" s="64"/>
-      <c r="S20" s="64"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="94"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="54"/>
+      <c r="R20" s="55"/>
+      <c r="S20" s="55"/>
       <c r="T20" s="30"/>
     </row>
     <row r="21" spans="1:20">
-      <c r="A21" s="48"/>
-      <c r="B21" s="97"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="98"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="46"/>
-      <c r="M21" s="46"/>
-      <c r="N21" s="46"/>
-      <c r="O21" s="46"/>
-      <c r="P21" s="46"/>
-      <c r="Q21" s="46"/>
-      <c r="R21" s="47"/>
-      <c r="S21" s="47"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="85"/>
+      <c r="I21" s="91"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="39"/>
+      <c r="S21" s="39"/>
       <c r="T21" s="30"/>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="48"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="53"/>
-      <c r="N22" s="53"/>
-      <c r="O22" s="53"/>
-      <c r="P22" s="53"/>
-      <c r="Q22" s="53"/>
-      <c r="R22" s="54"/>
-      <c r="S22" s="54"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="86"/>
+      <c r="I22" s="92"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="44"/>
+      <c r="Q22" s="44"/>
+      <c r="R22" s="45"/>
+      <c r="S22" s="45"/>
       <c r="T22" s="30"/>
     </row>
     <row r="23" spans="1:20">
-      <c r="A23" s="55"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="74"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="61"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="61"/>
-      <c r="N23" s="61"/>
-      <c r="O23" s="61"/>
-      <c r="P23" s="61"/>
-      <c r="Q23" s="61"/>
-      <c r="R23" s="62"/>
-      <c r="S23" s="62"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="93"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="52"/>
+      <c r="P23" s="52"/>
+      <c r="Q23" s="52"/>
+      <c r="R23" s="53"/>
+      <c r="S23" s="53"/>
       <c r="T23" s="30"/>
     </row>
     <row r="24" spans="1:20" s="1" customFormat="1">
-      <c r="A24" s="55"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="75"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="63"/>
-      <c r="K24" s="63"/>
-      <c r="L24" s="63"/>
-      <c r="M24" s="63"/>
-      <c r="N24" s="63"/>
-      <c r="O24" s="63"/>
-      <c r="P24" s="63"/>
-      <c r="Q24" s="63"/>
-      <c r="R24" s="64"/>
-      <c r="S24" s="64"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="94"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
+      <c r="O24" s="54"/>
+      <c r="P24" s="54"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="55"/>
+      <c r="S24" s="55"/>
     </row>
     <row r="25" spans="1:20" s="1" customFormat="1">
-      <c r="A25" s="48"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="46"/>
-      <c r="P25" s="46"/>
-      <c r="Q25" s="46"/>
-      <c r="R25" s="47"/>
-      <c r="S25" s="47"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="91"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
+      <c r="P25" s="34"/>
+      <c r="Q25" s="34"/>
+      <c r="R25" s="39"/>
+      <c r="S25" s="39"/>
     </row>
     <row r="26" spans="1:20" s="1" customFormat="1">
-      <c r="A26" s="48"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="53"/>
-      <c r="N26" s="53"/>
-      <c r="O26" s="53"/>
-      <c r="P26" s="53"/>
-      <c r="Q26" s="53"/>
-      <c r="R26" s="54"/>
-      <c r="S26" s="54"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="86"/>
+      <c r="I26" s="92"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
+      <c r="P26" s="44"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="45"/>
+      <c r="S26" s="45"/>
     </row>
     <row r="27" spans="1:20">
-      <c r="A27" s="55"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="60"/>
-      <c r="H27" s="74"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="61"/>
-      <c r="M27" s="61"/>
-      <c r="N27" s="61"/>
-      <c r="O27" s="61"/>
-      <c r="P27" s="61"/>
-      <c r="Q27" s="61"/>
-      <c r="R27" s="62"/>
-      <c r="S27" s="62"/>
+      <c r="A27" s="46"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="93"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="52"/>
+      <c r="N27" s="52"/>
+      <c r="O27" s="52"/>
+      <c r="P27" s="52"/>
+      <c r="Q27" s="52"/>
+      <c r="R27" s="53"/>
+      <c r="S27" s="53"/>
     </row>
     <row r="28" spans="1:20">
-      <c r="A28" s="67"/>
-      <c r="B28" s="68"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="63"/>
-      <c r="J28" s="63"/>
-      <c r="K28" s="63"/>
-      <c r="L28" s="63"/>
-      <c r="M28" s="63"/>
-      <c r="N28" s="63"/>
-      <c r="O28" s="63"/>
-      <c r="P28" s="63"/>
-      <c r="Q28" s="63"/>
-      <c r="R28" s="64"/>
-      <c r="S28" s="64"/>
+      <c r="A28" s="59"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="88"/>
+      <c r="I28" s="94"/>
+      <c r="J28" s="54"/>
+      <c r="K28" s="54"/>
+      <c r="L28" s="54"/>
+      <c r="M28" s="54"/>
+      <c r="N28" s="54"/>
+      <c r="O28" s="54"/>
+      <c r="P28" s="54"/>
+      <c r="Q28" s="54"/>
+      <c r="R28" s="55"/>
+      <c r="S28" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="A4:S4"/>
@@ -1735,24 +1721,12 @@
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="H23:H24"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"ＭＳ ゴシック,標準"&amp;7勤次郎株式会社&amp;C&amp;"ＭＳ ゴシック,太字"&amp;12振休確認表(日数管理_紐付あり_年月日)&amp;R&amp;"ＭＳ ゴシック,標準"&amp;7&amp;D　&amp;T　
+    <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;7勤次郎株式会社&amp;C&amp;"ＭＳ ゴシック,Regular"&amp;12振休確認表(日数管理_紐付あり_年月日)&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;7&amp;D　&amp;T　
 page&amp;P</oddHeader>
   </headerFooter>
 </worksheet>

</xml_diff>

<commit_message>
fix bug kdr003 #121388  #121390
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KDR003_template.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KDR003_template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7815"/>
   </bookViews>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -699,6 +704,48 @@
     <xf numFmtId="49" fontId="2" fillId="5" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -749,48 +796,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -802,6 +807,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1064,7 +1072,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" workbookViewId="0"/>
@@ -1074,8 +1082,8 @@
     <col min="1" max="1" width="3.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.25" style="2" customWidth="1"/>
     <col min="3" max="7" width="5.875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="2.5" style="90" customWidth="1"/>
-    <col min="9" max="9" width="5.125" style="90" customWidth="1"/>
+    <col min="8" max="8" width="2.5" style="65" customWidth="1"/>
+    <col min="9" max="9" width="5.125" style="65" customWidth="1"/>
     <col min="10" max="19" width="7.875" style="3" customWidth="1"/>
     <col min="20" max="20" width="9" style="1"/>
     <col min="21" max="16384" width="9" style="2"/>
@@ -1089,83 +1097,83 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
     </row>
     <row r="2" spans="1:20" ht="11.25" customHeight="1">
-      <c r="A2" s="69"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
-      <c r="S2" s="83"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="76"/>
+      <c r="S2" s="74"/>
       <c r="T2" s="30"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="70"/>
-      <c r="B3" s="72"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="82"/>
-      <c r="Q3" s="82"/>
-      <c r="R3" s="82"/>
-      <c r="S3" s="84"/>
+      <c r="A3" s="84"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="77"/>
+      <c r="S3" s="75"/>
       <c r="T3" s="30"/>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="66"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="68"/>
+      <c r="A4" s="80"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="82"/>
       <c r="T4" s="30"/>
     </row>
     <row r="5" spans="1:20">
@@ -1440,8 +1448,8 @@
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="42"/>
-      <c r="H17" s="85"/>
-      <c r="I17" s="91"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="66"/>
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
       <c r="L17" s="34"/>
@@ -1462,8 +1470,8 @@
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
       <c r="G18" s="43"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="92"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="67"/>
       <c r="J18" s="44"/>
       <c r="K18" s="44"/>
       <c r="L18" s="44"/>
@@ -1484,8 +1492,8 @@
       <c r="E19" s="49"/>
       <c r="F19" s="50"/>
       <c r="G19" s="51"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="93"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="68"/>
       <c r="J19" s="52"/>
       <c r="K19" s="52"/>
       <c r="L19" s="52"/>
@@ -1506,8 +1514,8 @@
       <c r="E20" s="49"/>
       <c r="F20" s="50"/>
       <c r="G20" s="51"/>
-      <c r="H20" s="88"/>
-      <c r="I20" s="94"/>
+      <c r="H20" s="73"/>
+      <c r="I20" s="69"/>
       <c r="J20" s="54"/>
       <c r="K20" s="54"/>
       <c r="L20" s="54"/>
@@ -1528,8 +1536,8 @@
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
       <c r="G21" s="57"/>
-      <c r="H21" s="85"/>
-      <c r="I21" s="91"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="66"/>
       <c r="J21" s="34"/>
       <c r="K21" s="34"/>
       <c r="L21" s="34"/>
@@ -1550,8 +1558,8 @@
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="43"/>
-      <c r="H22" s="86"/>
-      <c r="I22" s="92"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="67"/>
       <c r="J22" s="44"/>
       <c r="K22" s="44"/>
       <c r="L22" s="44"/>
@@ -1572,8 +1580,8 @@
       <c r="E23" s="49"/>
       <c r="F23" s="50"/>
       <c r="G23" s="51"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="93"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="68"/>
       <c r="J23" s="52"/>
       <c r="K23" s="52"/>
       <c r="L23" s="52"/>
@@ -1594,8 +1602,8 @@
       <c r="E24" s="49"/>
       <c r="F24" s="50"/>
       <c r="G24" s="51"/>
-      <c r="H24" s="88"/>
-      <c r="I24" s="94"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="69"/>
       <c r="J24" s="54"/>
       <c r="K24" s="54"/>
       <c r="L24" s="54"/>
@@ -1615,8 +1623,8 @@
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
       <c r="G25" s="21"/>
-      <c r="H25" s="85"/>
-      <c r="I25" s="91"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="66"/>
       <c r="J25" s="34"/>
       <c r="K25" s="34"/>
       <c r="L25" s="34"/>
@@ -1636,8 +1644,8 @@
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="21"/>
-      <c r="H26" s="86"/>
-      <c r="I26" s="92"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="67"/>
       <c r="J26" s="44"/>
       <c r="K26" s="44"/>
       <c r="L26" s="44"/>
@@ -1657,8 +1665,8 @@
       <c r="E27" s="50"/>
       <c r="F27" s="50"/>
       <c r="G27" s="51"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="93"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="68"/>
       <c r="J27" s="52"/>
       <c r="K27" s="52"/>
       <c r="L27" s="52"/>
@@ -1678,8 +1686,8 @@
       <c r="E28" s="62"/>
       <c r="F28" s="62"/>
       <c r="G28" s="63"/>
-      <c r="H28" s="88"/>
-      <c r="I28" s="94"/>
+      <c r="H28" s="73"/>
+      <c r="I28" s="69"/>
       <c r="J28" s="54"/>
       <c r="K28" s="54"/>
       <c r="L28" s="54"/>
@@ -1693,18 +1701,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="A4:S4"/>
@@ -1721,9 +1717,21 @@
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="H23:H24"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;7勤次郎株式会社&amp;C&amp;"ＭＳ ゴシック,Regular"&amp;12振休確認表(日数管理_紐付あり_年月日)&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;7&amp;D　&amp;T　

</xml_diff>